<commit_message>
improve import trucks from excel
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportTrucksSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportTrucksSampleFile.xlsx
@@ -1,71 +1,109 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A22E533-56E6-4F0E-8130-9433604E90EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F495E8-DF58-4587-867C-C11A12D45B69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="iZDSbPe2E80itPOZg6Io+rwIfsBn2AK8J+7BNzOZdf0+VcqLNAXi+c3guhUpAsk3lqc/n5aXlfOTBwnyi9yg3g==" workbookSaltValue="J0fIIt/EKCJHn6UCa3xByg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Trucks" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+  <si>
+    <t>Model year</t>
+  </si>
+  <si>
+    <t>Is attachable</t>
+  </si>
   <si>
     <t>Note</t>
   </si>
   <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>TruckStatusId</t>
-  </si>
-  <si>
-    <t>IsAttachable</t>
-  </si>
-  <si>
-    <t>ModelYear</t>
-  </si>
-  <si>
-    <t>ModelName</t>
-  </si>
-  <si>
-    <t>PlateNumber</t>
-  </si>
-  <si>
-    <t>Driver1UserId</t>
-  </si>
-  <si>
-    <t>TransportTypeId</t>
-  </si>
-  <si>
-    <t>TransportSubtypeId</t>
-  </si>
-  <si>
-    <t>TrucksTypeId</t>
-  </si>
-  <si>
-    <t>TruckSubtypeId</t>
-  </si>
-  <si>
-    <t>CapacityId</t>
+    <t>Truck Subtype</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Istimara NO*</t>
+  </si>
+  <si>
+    <t>Model Name</t>
+  </si>
+  <si>
+    <t>Insurance Policy NO*</t>
+  </si>
+  <si>
+    <t>Capacity (Payload)*</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Istimara Expiry  Date (Gregorian)*</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Istimara Expiry  Date (Hijri)*</t>
+  </si>
+  <si>
+    <t>Insurance Expiry Date (Hijri)*</t>
+  </si>
+  <si>
+    <t>Insurance Expiry Date (Gregorian)*</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Plate NO*</t>
+  </si>
+  <si>
+    <t>Transport Type*</t>
+  </si>
+  <si>
+    <t>Transport Subtype</t>
+  </si>
+  <si>
+    <t>Truck Type</t>
+  </si>
+  <si>
+    <t>Frozen</t>
+  </si>
+  <si>
+    <t>Cold Chain</t>
+  </si>
+  <si>
+    <t>Freezer Dyana &amp; Smaller Capacities</t>
+  </si>
+  <si>
+    <t>islam</t>
+  </si>
+  <si>
+    <t>30/4/1442</t>
+  </si>
+  <si>
+    <t>26/11/2020</t>
+  </si>
+  <si>
+    <t>islam test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-1170000]B2dd/mm/yyyy;@"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -74,23 +112,37 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
+      <b/>
+      <sz val="9"/>
+      <name val="Open Sans"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
+      <b/>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Open Sans"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -105,13 +157,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,146 +499,168 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{017B1AF8-713B-4EA9-A51A-392997C3CF5A}">
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="12.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="24.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:16" s="2" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="O1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="P1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="3">
         <v>123</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="3">
         <v>123</v>
       </c>
-      <c r="C2" s="3">
-        <v>2000</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3">
-        <v>123</v>
-      </c>
-      <c r="F2" s="3">
-        <v>3</v>
-      </c>
-      <c r="G2" s="3">
-        <v>6</v>
-      </c>
-      <c r="H2" s="3">
-        <v>1</v>
-      </c>
-      <c r="I2" s="3">
-        <v>3</v>
-      </c>
-      <c r="J2" s="3">
-        <v>10</v>
-      </c>
-      <c r="K2" s="3">
-        <v>3</v>
-      </c>
-      <c r="L2" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>123</v>
-      </c>
-      <c r="B3" s="3">
-        <v>123</v>
-      </c>
-      <c r="C3" s="3">
-        <v>2001</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3">
-        <v>124</v>
-      </c>
-      <c r="F3" s="3">
-        <v>3</v>
-      </c>
-      <c r="G3" s="3">
-        <v>6</v>
-      </c>
-      <c r="H3" s="3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3">
-        <v>3</v>
-      </c>
-      <c r="J3" s="3">
-        <v>10</v>
-      </c>
-      <c r="K3" s="3">
-        <v>3</v>
-      </c>
-      <c r="L3" s="3">
-        <v>3</v>
+      <c r="L2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="3">
+        <v>222</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="22">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does it have a trailer" sqref="D1" xr:uid="{C110D44F-E18D-4F5D-93BF-E889364073BE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="What is the transport type of this truck , Please select one from the list (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="E1" xr:uid="{0D4FDBC6-9967-4FA9-A93F-81A3D88BB043}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please skip this if transport type not (Cold Chain), if yes pleas select one from the list " sqref="F1" xr:uid="{2AA161EE-20A7-4B46-97B3-FAD0D572E0A7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the truck type from the list (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="G1" xr:uid="{7AC6C272-AB1D-465B-A457-A9F06996B9EB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please skip this if truck type not (Dyana), if yes please select one from the list " sqref="H1" xr:uid="{7259F8EC-91AE-467B-B8B3-666E1B7B977C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add truck plate number (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="A1:A1048576" xr:uid="{E202FB0B-CA72-439B-B622-885177E5DB1B}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="What is the transport type of this truck , Please select one from the list. (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="E2:E1048576" xr:uid="{8EBD1E04-C6C6-4B32-9A02-F8D3D9558F80}">
+      <formula1>"Ambient,Cold Chain,Others"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the truck type from the list (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="G2:G1048576" xr:uid="{D0CB12CA-C2E6-4349-AE25-636E8DEBD95B}">
+      <formula1>"Flatbed,Dyana,Closed Box,Curtain Sides,Sidewall,Open Top,Car Shuttler,Genset,Closed Box Reefer,Reefer Dyana &amp; Smaller Capacity,Closed Box Freezer,Freezer Dyana &amp; Smaller Capacities,Others"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please skip this if transport type not (Cold Chain), if yes pleas select one from the list " sqref="F3:F1048576" xr:uid="{B769D09A-4F62-48CF-A2E0-137E4F3F7686}">
+      <formula1>"Temp Controlled,Frozen "</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please skip this if truck type not (Dyana), if yes please select one from the list " sqref="H2:H1048576" xr:uid="{22BB5121-8A85-457D-8264-617389BC5576}">
+      <formula1>"Closed Box,Open Top"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add truck model name " sqref="B1:B1048576" xr:uid="{0ABC31F2-DEB2-4183-8B98-257FE8609CDA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add truck model year " sqref="C1:C1048576" xr:uid="{0B1D9562-4932-4256-86C5-BD750603F713}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does it have a trailer" sqref="D2:D1048576" xr:uid="{58369A68-2077-4A8F-9C0D-03E6586E803F}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please enter the payload of this truck in Tonnage (Note: this is a mandatory field, your file will be rejectd if this field is empty)" sqref="I1:I1048576" xr:uid="{6EE8D2D0-F9A4-43E6-967D-FAA6C0B2C490}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add any additonal information about this truck. " sqref="J1:J1048576" xr:uid="{8DE2E6CD-719B-4EBE-8FA6-9D9AF0DE08A5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add truck Istimara number (Note: this is a mandatory field, your file will be rejectd if this field is empty)" sqref="K1:K1048576" xr:uid="{3835016D-50DD-441E-B453-02F844673B86}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add Istimara expiration date, you can enter the date in Gregorian or Hijri, in this field please use Gregorian date: DD/MM/YYYY (Note: this is a mandatory field, your file will be rejectd if this field is empty)" sqref="M1:M1048576 P2" xr:uid="{2B424BB8-BD57-403A-9C17-C6799B73FE45}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add 3rd party insurance number (Note: this is a mandatory field, your file will be rejectd if this field is empty)" sqref="N1:N1048576" xr:uid="{D76BE6A7-1590-451C-9BEA-3A8AE4EF8F19}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add Istimara expiration date, you can enter the date in Gregorian or Hijri, in this field please use Hijri date: DD/MM/YYYY (Note: this is a mandatory field, your file will be rejectd if this field is empty)" sqref="L1:L1048576 O2" xr:uid="{CF6393D9-FA5F-422E-AB53-B3D68BCE1238}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add the expiration date for the 3rd Party Insurance, you can enter the date in Gregorian or Hijri, in this field please use Hijri date: DD/MM/YYYY (Note: this is a mandatory field, your file will be reject if this field is empty)" sqref="O1 O3:O1048576" xr:uid="{F353D8D7-9393-48AB-A5AE-0889A44B0F47}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add the expiration date for the 3rd Party Insurance, you can enter the date in Gregorian or Hijri, in this field please use Gregorian date: DD/MM/YYYY (Note: this is a mandatory field, your file will be reject if this field is empty)" sqref="P1 P3:P1048576" xr:uid="{FDF31937-D4D0-45BA-B19C-7C9EFFE920D8}"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="Please skip this if transport type not (Cold Chain), if yes pleas select one from the list " sqref="F2" xr:uid="{F254450F-1FC6-4D0A-A1F1-A74D5972B543}">
+      <formula1>"Temp Controlled,Frozen, "</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
#816  Improve import truck from excel
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportTrucksSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportTrucksSampleFile.xlsx
@@ -5,13 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Trucks &amp; Drivers\Trucks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F495E8-DF58-4587-867C-C11A12D45B69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="iZDSbPe2E80itPOZg6Io+rwIfsBn2AK8J+7BNzOZdf0+VcqLNAXi+c3guhUpAsk3lqc/n5aXlfOTBwnyi9yg3g==" workbookSaltValue="J0fIIt/EKCJHn6UCa3xByg==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA328C2-BD00-4106-BC35-922C664D3FCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trucks" sheetId="2" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Model year</t>
   </si>
@@ -29,81 +28,53 @@
     <t>Is attachable</t>
   </si>
   <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>Truck Subtype</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Istimara NO*</t>
+    <t xml:space="preserve">Truck Type* </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plate NO* </t>
   </si>
   <si>
     <t>Model Name</t>
   </si>
   <si>
-    <t>Insurance Policy NO*</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport Type* </t>
   </si>
   <si>
     <t>Capacity (Payload)*</t>
   </si>
   <si>
-    <t xml:space="preserve"> Istimara Expiry  Date (Gregorian)*</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Istimara Expiry  Date (Hijri)*</t>
-  </si>
-  <si>
-    <t>Insurance Expiry Date (Hijri)*</t>
-  </si>
-  <si>
-    <t>Insurance Expiry Date (Gregorian)*</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Plate NO*</t>
-  </si>
-  <si>
-    <t>Transport Type*</t>
-  </si>
-  <si>
-    <t>Transport Subtype</t>
-  </si>
-  <si>
-    <t>Truck Type</t>
-  </si>
-  <si>
-    <t>Frozen</t>
-  </si>
-  <si>
-    <t>Cold Chain</t>
-  </si>
-  <si>
-    <t>Freezer Dyana &amp; Smaller Capacities</t>
-  </si>
-  <si>
-    <t>islam</t>
-  </si>
-  <si>
-    <t>30/4/1442</t>
-  </si>
-  <si>
-    <t>26/11/2020</t>
-  </si>
-  <si>
-    <t>islam test</t>
+    <t xml:space="preserve"> Istimara Expiry  Date (Gregorian)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Istimara Expiry  Date (Hijri)</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3rd party Insurance Expiry Date (Hijri)</t>
+  </si>
+  <si>
+    <t>3rd Party Insurance Policy NO*</t>
+  </si>
+  <si>
+    <t>3rd party Insurance Expiry Date (Gregorian)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Truck length </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Istimara/Sequence NO*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
-    <numFmt numFmtId="165" formatCode="[$-1170000]B2dd/mm/yyyy;@"/>
-  </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -125,7 +96,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,18 +105,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -153,38 +118,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -500,168 +468,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{017B1AF8-713B-4EA9-A51A-392997C3CF5A}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.28515625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="24.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.7109375" style="3"/>
+    <col min="1" max="1" width="12.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.453125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="24.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="28" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="36.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="3">
-        <v>123</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="3">
-        <v>2020</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="3">
-        <v>2</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="3">
-        <v>123</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="3">
-        <v>222</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>22</v>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="22">
+  <sheetProtection algorithmName="SHA-512" hashValue="9B3CH8xf2qBlqkaDCwVzEjHeHKOuF1TnmnaHwUqgxFgHIAJ2F5RUQhHVHmUzRhW+BBqivtwg96SI0uTu3ahEYg==" saltValue="/Q/5oTP4bfSQiRca1T4QGA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <dataValidations count="18">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add truck plate number (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="A1" xr:uid="{E202FB0B-CA72-439B-B622-885177E5DB1B}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{8EBD1E04-C6C6-4B32-9A02-F8D3D9558F80}">
+      <formula1>"Ambient,Cold Chain,Others"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add truck model name " sqref="B1" xr:uid="{0ABC31F2-DEB2-4183-8B98-257FE8609CDA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add truck model year " sqref="C1" xr:uid="{0B1D9562-4932-4256-86C5-BD750603F713}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{58369A68-2077-4A8F-9C0D-03E6586E803F}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does it have a trailer" sqref="D1" xr:uid="{C110D44F-E18D-4F5D-93BF-E889364073BE}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="What is the transport type of this truck , Please select one from the list (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="E1" xr:uid="{0D4FDBC6-9967-4FA9-A93F-81A3D88BB043}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please skip this if transport type not (Cold Chain), if yes pleas select one from the list " sqref="F1" xr:uid="{2AA161EE-20A7-4B46-97B3-FAD0D572E0A7}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the truck type from the list (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="G1" xr:uid="{7AC6C272-AB1D-465B-A457-A9F06996B9EB}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please skip this if truck type not (Dyana), if yes please select one from the list " sqref="H1" xr:uid="{7259F8EC-91AE-467B-B8B3-666E1B7B977C}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add truck plate number (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="A1:A1048576" xr:uid="{E202FB0B-CA72-439B-B622-885177E5DB1B}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="What is the transport type of this truck , Please select one from the list. (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="E2:E1048576" xr:uid="{8EBD1E04-C6C6-4B32-9A02-F8D3D9558F80}">
-      <formula1>"Ambient,Cold Chain,Others"</formula1>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the truck type from the list (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="F1" xr:uid="{7AC6C272-AB1D-465B-A457-A9F06996B9EB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please enter the payload of this truck in Tonnage (Note: this is a mandatory field, your file will be rejectd if this field is empty)" sqref="H1" xr:uid="{6EE8D2D0-F9A4-43E6-967D-FAA6C0B2C490}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add any additonal information about this truck. " sqref="I1" xr:uid="{8DE2E6CD-719B-4EBE-8FA6-9D9AF0DE08A5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add truck Istimara number (Note: this is a mandatory field, your file will be rejectd if this field is empty)" sqref="J1" xr:uid="{3835016D-50DD-441E-B453-02F844673B86}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add Istimara expiration date, either Hijri or Gregorian dates (Note: in this field please use Hijri, date: DD/MM/YYYY )" sqref="K1" xr:uid="{CF6393D9-FA5F-422E-AB53-B3D68BCE1238}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{81C1232D-02CA-40FC-ADEE-EAF959CD4E5F}">
+      <formula1>"Flatbed,Closed box trailer,Curtain sides trailer,Sidewall trailer,Open top,Dyana Closed box,Dyana Open top,Pick up,Car Shuttler,Lowbed,Genset,Reefer Truck,Reefer Dyana,Reefer pick up,Freezer Truck,Freezer Dyana,Freezer pick up,Others"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the truck type from the list (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="G2:G1048576" xr:uid="{D0CB12CA-C2E6-4349-AE25-636E8DEBD95B}">
-      <formula1>"Flatbed,Dyana,Closed Box,Curtain Sides,Sidewall,Open Top,Car Shuttler,Genset,Closed Box Reefer,Reefer Dyana &amp; Smaller Capacity,Closed Box Freezer,Freezer Dyana &amp; Smaller Capacities,Others"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please skip this if transport type not (Cold Chain), if yes pleas select one from the list " sqref="F3:F1048576" xr:uid="{B769D09A-4F62-48CF-A2E0-137E4F3F7686}">
-      <formula1>"Temp Controlled,Frozen "</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please skip this if truck type not (Dyana), if yes please select one from the list " sqref="H2:H1048576" xr:uid="{22BB5121-8A85-457D-8264-617389BC5576}">
-      <formula1>"Closed Box,Open Top"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add truck model name " sqref="B1:B1048576" xr:uid="{0ABC31F2-DEB2-4183-8B98-257FE8609CDA}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add truck model year " sqref="C1:C1048576" xr:uid="{0B1D9562-4932-4256-86C5-BD750603F713}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Does it have a trailer" sqref="D2:D1048576" xr:uid="{58369A68-2077-4A8F-9C0D-03E6586E803F}">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please enter the payload of this truck in Tonnage (Note: this is a mandatory field, your file will be rejectd if this field is empty)" sqref="I1:I1048576" xr:uid="{6EE8D2D0-F9A4-43E6-967D-FAA6C0B2C490}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add any additonal information about this truck. " sqref="J1:J1048576" xr:uid="{8DE2E6CD-719B-4EBE-8FA6-9D9AF0DE08A5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add truck Istimara number (Note: this is a mandatory field, your file will be rejectd if this field is empty)" sqref="K1:K1048576" xr:uid="{3835016D-50DD-441E-B453-02F844673B86}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add Istimara expiration date, you can enter the date in Gregorian or Hijri, in this field please use Gregorian date: DD/MM/YYYY (Note: this is a mandatory field, your file will be rejectd if this field is empty)" sqref="M1:M1048576 P2" xr:uid="{2B424BB8-BD57-403A-9C17-C6799B73FE45}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add 3rd party insurance number (Note: this is a mandatory field, your file will be rejectd if this field is empty)" sqref="N1:N1048576" xr:uid="{D76BE6A7-1590-451C-9BEA-3A8AE4EF8F19}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add Istimara expiration date, you can enter the date in Gregorian or Hijri, in this field please use Hijri date: DD/MM/YYYY (Note: this is a mandatory field, your file will be rejectd if this field is empty)" sqref="L1:L1048576 O2" xr:uid="{CF6393D9-FA5F-422E-AB53-B3D68BCE1238}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add the expiration date for the 3rd Party Insurance, you can enter the date in Gregorian or Hijri, in this field please use Hijri date: DD/MM/YYYY (Note: this is a mandatory field, your file will be reject if this field is empty)" sqref="O1 O3:O1048576" xr:uid="{F353D8D7-9393-48AB-A5AE-0889A44B0F47}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add the expiration date for the 3rd Party Insurance, you can enter the date in Gregorian or Hijri, in this field please use Gregorian date: DD/MM/YYYY (Note: this is a mandatory field, your file will be reject if this field is empty)" sqref="P1 P3:P1048576" xr:uid="{FDF31937-D4D0-45BA-B19C-7C9EFFE920D8}"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="Please skip this if transport type not (Cold Chain), if yes pleas select one from the list " sqref="F2" xr:uid="{F254450F-1FC6-4D0A-A1F1-A74D5972B543}">
-      <formula1>"Temp Controlled,Frozen, "</formula1>
-    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add the expiration date for the 3rd Party Insurance, either Hijri or Gregorian dates (Note: in this field please use Gregorian date: DD/MM/YYYY )" sqref="O1" xr:uid="{FDF31937-D4D0-45BA-B19C-7C9EFFE920D8}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add the expiration date for the 3rd Party Insurance, either Hijri or Gregorian dates (Note: in this field please use Hijri date: DD/MM/YYYY )" sqref="N1" xr:uid="{F353D8D7-9393-48AB-A5AE-0889A44B0F47}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add 3rd party insurance number (Note: this is a mandatory field, your file will be rejectd if this field is empty)" sqref="M1" xr:uid="{D76BE6A7-1590-451C-9BEA-3A8AE4EF8F19}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add Istimara expiration date, either Hijri or Gregorian dates (Note: in this field please use Gregorian date: DD/MM/YYYY )" sqref="L1" xr:uid="{2B424BB8-BD57-403A-9C17-C6799B73FE45}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please enter truck lenght in Meter " sqref="G1" xr:uid="{C2046C24-D300-4759-8677-6CC20644EB40}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Import trucks from excel sample file
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportTrucksSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportTrucksSampleFile.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\source\tachyon-core\angular\src\assets\sampleFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A14DD87-3C56-4A7B-BBC3-FE46BC5E0B23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D05629F-E513-4F4A-809C-05FC1C5AE8C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3043" windowWidth="26219" windowHeight="8110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="21954" windowHeight="11982" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trucks" sheetId="2" r:id="rId1"/>
+    <sheet name="Lists" sheetId="3" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="TransportTypes">Lists!$A$2:$A$4</definedName>
+    <definedName name="TruckTypes">Lists!$B$2:$B$24</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>Model year</t>
   </si>
@@ -68,13 +73,91 @@
   </si>
   <si>
     <t xml:space="preserve"> Istimara/Sequence NO*</t>
+  </si>
+  <si>
+    <t>Truck Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport Type </t>
+  </si>
+  <si>
+    <t>Flatbed</t>
+  </si>
+  <si>
+    <t>Closed box trailer</t>
+  </si>
+  <si>
+    <t>Curtain sides trailer</t>
+  </si>
+  <si>
+    <t>Sidewall trailer</t>
+  </si>
+  <si>
+    <t>Van</t>
+  </si>
+  <si>
+    <t>Open Pick Up</t>
+  </si>
+  <si>
+    <t>Open Top</t>
+  </si>
+  <si>
+    <t>Dyana Closed Box</t>
+  </si>
+  <si>
+    <t>Dyana Open Top</t>
+  </si>
+  <si>
+    <t>Closed Pick Up</t>
+  </si>
+  <si>
+    <t>Genset</t>
+  </si>
+  <si>
+    <t>Reefer Truck 15C-25C</t>
+  </si>
+  <si>
+    <t>Reefer Dyana 15C-25C</t>
+  </si>
+  <si>
+    <t>Reefer Pick Up 15C-25C</t>
+  </si>
+  <si>
+    <t>Freezer Truck -20C - 0C</t>
+  </si>
+  <si>
+    <t>Freezer Dyana -20C - 0C</t>
+  </si>
+  <si>
+    <t>Freezer Pick Up -20C - 0C</t>
+  </si>
+  <si>
+    <t>Chiller Truck 0C - 8C</t>
+  </si>
+  <si>
+    <t>Chiller Dyana 0C - 8C</t>
+  </si>
+  <si>
+    <t>Chiller Pick Up 0C - 8C</t>
+  </si>
+  <si>
+    <t>Tanker</t>
+  </si>
+  <si>
+    <t>Special Tanker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Others </t>
+  </si>
+  <si>
+    <t>Ambient</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -92,6 +175,25 @@
       <b/>
       <sz val="9"/>
       <color indexed="8"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Poppins"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Open Sans"/>
       <family val="2"/>
     </font>
@@ -137,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -155,6 +257,24 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +592,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.3"/>
@@ -540,11 +660,6 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="4" spans="1:15">
       <c r="A4" s="5" t="s">
         <v>5</v>
@@ -584,7 +699,7 @@
   <dataValidations count="18">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add truck plate number (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="A1" xr:uid="{E202FB0B-CA72-439B-B622-885177E5DB1B}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{8EBD1E04-C6C6-4B32-9A02-F8D3D9558F80}">
-      <formula1>"Ambient,Cold Chain,Others"</formula1>
+      <formula1>TransportTypes</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add truck model name " sqref="B1" xr:uid="{0ABC31F2-DEB2-4183-8B98-257FE8609CDA}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add truck model year " sqref="C1" xr:uid="{0B1D9562-4932-4256-86C5-BD750603F713}"/>
@@ -599,7 +714,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add truck Istimara number (Note: this is a mandatory field, your file will be rejectd if this field is empty)" sqref="J1" xr:uid="{3835016D-50DD-441E-B453-02F844673B86}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add Istimara expiration date, either Hijri or Gregorian dates (Note: in this field please use Hijri, date: DD/MM/YYYY )" sqref="K1" xr:uid="{CF6393D9-FA5F-422E-AB53-B3D68BCE1238}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{81C1232D-02CA-40FC-ADEE-EAF959CD4E5F}">
-      <formula1>"Flatbed,Closed box trailer,Curtain sides trailer,Sidewall trailer,Open top,Dyana Closed box,Dyana Open top,Pick up,Car Shuttler,Lowbed,Genset,Reefer Truck,Reefer Dyana,Reefer pick up,Freezer Truck,Freezer Dyana,Freezer pick up,Others"</formula1>
+      <formula1>TruckTypes</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add the expiration date for the 3rd Party Insurance, either Hijri or Gregorian dates (Note: in this field please use Gregorian date: DD/MM/YYYY )" sqref="O1" xr:uid="{FDF31937-D4D0-45BA-B19C-7C9EFFE920D8}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add the expiration date for the 3rd Party Insurance, either Hijri or Gregorian dates (Note: in this field please use Hijri date: DD/MM/YYYY )" sqref="N1" xr:uid="{F353D8D7-9393-48AB-A5AE-0889A44B0F47}"/>
@@ -610,4 +725,177 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3032A858-A5B4-4C8B-8DB0-CCB33CB3AF1A}">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.3"/>
+  <cols>
+    <col min="1" max="1" width="21.875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="20" style="7" customWidth="1"/>
+    <col min="3" max="16384" width="8.75" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="12"/>
+      <c r="B12" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="12"/>
+      <c r="B14" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="12"/>
+      <c r="B15" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="12"/>
+      <c r="B16" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="12"/>
+      <c r="B17" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="12"/>
+      <c r="B20" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="12"/>
+      <c r="B21" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="8"/>
+      <c r="B24" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Edit import truck from excel sample files
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportTrucksSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportTrucksSampleFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D05629F-E513-4F4A-809C-05FC1C5AE8C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DA7117-F046-41C8-A327-50A28C0D73DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="21954" windowHeight="11982" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Lists" sheetId="3" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="TransportTypes">Lists!$A$2:$A$4</definedName>
+    <definedName name="TransportTypes">Lists!$A$2:$A$5</definedName>
     <definedName name="TruckTypes">Lists!$B$2:$B$24</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>Model year</t>
   </si>
@@ -151,13 +151,19 @@
   </si>
   <si>
     <t>Ambient</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Cold Chain</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -196,6 +202,13 @@
       <color rgb="FFFFFFFF"/>
       <name val="Open Sans"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -239,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -275,6 +288,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,7 +606,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.3"/>
@@ -732,7 +746,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B24"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.3"/>
@@ -759,8 +773,8 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="8" t="s">
-        <v>38</v>
+      <c r="A3" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>19</v>
@@ -768,14 +782,16 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="8"/>
+      <c r="A5" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="B5" s="9" t="s">
         <v>21</v>
       </c>
@@ -896,6 +912,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TAC-238 Add (Car Shuttler & Lowbed) as a truck type to the excel file
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportTrucksSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportTrucksSampleFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mosa Alhaj\source\repos\tachyon-core\angular\src\assets\sampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DA7117-F046-41C8-A327-50A28C0D73DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCF8651-F26C-4AA7-B4F1-4D9F2BDF3760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="21954" windowHeight="11982" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2892" yWindow="2892" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trucks" sheetId="2" r:id="rId1"/>
@@ -18,14 +18,14 @@
   </sheets>
   <definedNames>
     <definedName name="TransportTypes">Lists!$A$2:$A$5</definedName>
-    <definedName name="TruckTypes">Lists!$B$2:$B$24</definedName>
+    <definedName name="TruckTypes">Lists!$B$2:$B$26</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>Model year</t>
   </si>
@@ -157,13 +157,19 @@
   </si>
   <si>
     <t>Cold Chain</t>
+  </si>
+  <si>
+    <t>Lowbed</t>
+  </si>
+  <si>
+    <t>Car Shuttler</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -606,28 +612,28 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="21.125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="16.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5" style="5" customWidth="1"/>
-    <col min="9" max="9" width="24.25" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.44140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="24.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.88671875" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="28" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="32" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="36.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.75" style="5"/>
+    <col min="14" max="15" width="36.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="4" customFormat="1" ht="11.55">
+    <row r="1" spans="1:15" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -674,37 +680,37 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
@@ -743,20 +749,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3032A858-A5B4-4C8B-8DB0-CCB33CB3AF1A}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.875" style="11" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" style="11" customWidth="1"/>
     <col min="2" max="2" width="20" style="7" customWidth="1"/>
-    <col min="3" max="16384" width="8.75" style="7"/>
+    <col min="3" max="16384" width="8.77734375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>17</v>
       </c>
@@ -764,7 +770,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>41</v>
       </c>
@@ -772,7 +778,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>43</v>
       </c>
@@ -780,7 +786,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>38</v>
       </c>
@@ -788,7 +794,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>42</v>
       </c>
@@ -796,117 +802,127 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
       <c r="B12" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="B15" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
       <c r="B20" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
       <c r="B21" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B25" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B26" s="9" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>